<commit_message>
update format windows filename
</commit_message>
<xml_diff>
--- a/巡检模板.xlsx
+++ b/巡检模板.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="64">
   <si>
     <t>display current-configuration</t>
   </si>
@@ -279,10 +279,6 @@
   </si>
   <si>
     <t>192.168.0.11</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>#</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -923,7 +919,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomRight" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.59765625" defaultRowHeight="15.6"/>
@@ -980,6 +976,9 @@
         <v>61</v>
       </c>
       <c r="D2" s="3"/>
+      <c r="E2" s="1">
+        <v>22</v>
+      </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -990,13 +989,14 @@
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>62</v>
-      </c>
+      <c r="B3" s="3"/>
       <c r="C3" s="11" t="s">
         <v>54</v>
       </c>
       <c r="D3" s="3"/>
+      <c r="E3" s="1">
+        <v>22</v>
+      </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -1008,7 +1008,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>62</v>
+        <v>2</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>55</v>
@@ -1025,7 +1025,7 @@
         <v>13</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>62</v>
+        <v>2</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>56</v>
@@ -1042,7 +1042,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>62</v>
+        <v>2</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>57</v>
@@ -1059,10 +1059,10 @@
         <v>15</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>62</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>63</v>
       </c>
       <c r="D7" s="3"/>
       <c r="F7" s="3"/>
@@ -1076,10 +1076,10 @@
         <v>16</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>62</v>
+        <v>2</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D8" s="3"/>
       <c r="F8" s="3"/>
@@ -1093,7 +1093,7 @@
         <v>17</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>62</v>
+        <v>2</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>58</v>
@@ -1110,7 +1110,7 @@
         <v>18</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>62</v>
+        <v>2</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>59</v>
@@ -1127,7 +1127,7 @@
         <v>19</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>62</v>
+        <v>2</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>60</v>
@@ -1804,11 +1804,49 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_x6587__x6863__x72b6__x6001_ xmlns="5c1e9b2d-f6f5-4391-84fa-7715816b5f0f">初稿未完成</_x6587__x6863__x72b6__x6001_>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1976,49 +2014,11 @@
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_x6587__x6863__x72b6__x6001_ xmlns="5c1e9b2d-f6f5-4391-84fa-7715816b5f0f">初稿未完成</_x6587__x6863__x72b6__x6001_>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2030,18 +2030,9 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC99DC05-5E1F-4E6B-BF48-D75A6E6CB5B0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{075988A9-20C0-4BE8-A91F-94F7140E4C90}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="5c1e9b2d-f6f5-4391-84fa-7715816b5f0f"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="4b7a6e08-f856-4fbd-a92d-718f0ebb94c9"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2066,9 +2057,18 @@
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{075988A9-20C0-4BE8-A91F-94F7140E4C90}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC99DC05-5E1F-4E6B-BF48-D75A6E6CB5B0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="5c1e9b2d-f6f5-4391-84fa-7715816b5f0f"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="4b7a6e08-f856-4fbd-a92d-718f0ebb94c9"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>